<commit_message>
Changes for forecaster release 3.10.4
</commit_message>
<xml_diff>
--- a/schedules/Diphtheria.xlsx
+++ b/schedules/Diphtheria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="155">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -486,6 +486,9 @@
   </si>
   <si>
     <t xml:space="preserve">Patient received 3rd valid dose after 4 years of age, now expecting final DTaP booster. </t>
+  </si>
+  <si>
+    <t>123, 110, 114, 113, 115, 116, 121, 2060, 111, 2070</t>
   </si>
 </sst>
 </file>
@@ -1317,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1448,14 +1451,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9">
-        <v>123</v>
-      </c>
-      <c r="D8" s="44" t="s">
+      <c r="C8" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="48"/>
+      <c r="E8" s="44" t="s">
         <v>63</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1471,13 +1475,9 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="9">
-        <v>-110</v>
-      </c>
-      <c r="D9" s="42"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
       <c r="F9" s="9" t="s">
         <v>21</v>
       </c>
@@ -1492,12 +1492,12 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C10" s="9">
-        <v>-12</v>
-      </c>
-      <c r="D10" s="11"/>
+        <v>-110</v>
+      </c>
+      <c r="D10" s="42"/>
       <c r="F10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1512,10 +1512,10 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C11" s="9">
-        <v>-4</v>
+        <v>-12</v>
       </c>
       <c r="D11" s="11"/>
       <c r="F11" s="9" t="s">
@@ -1530,10 +1530,10 @@
     </row>
     <row r="12" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C12" s="9">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="D12" s="11"/>
       <c r="F12" s="9" t="s">
@@ -1547,6 +1547,13 @@
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-7</v>
+      </c>
+      <c r="D13" s="11"/>
       <c r="F13" s="9" t="s">
         <v>25</v>
       </c>
@@ -1558,11 +1565,6 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
       <c r="F14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1574,15 +1576,11 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>129</v>
-      </c>
+      <c r="B15" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="F15" s="9" t="s">
         <v>26</v>
       </c>
@@ -1594,14 +1592,14 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="12">
-        <v>-12</v>
+      <c r="B16" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>27</v>
@@ -1615,13 +1613,13 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D17" s="12">
-        <v>-4</v>
+        <v>-12</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>28</v>
@@ -1637,13 +1635,13 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D18" s="12">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>30</v>
@@ -1655,6 +1653,17 @@
       <c r="I18" s="11"/>
       <c r="J18" s="12">
         <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="12">
+        <v>-7</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
@@ -4597,14 +4606,18 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="34">
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B140:E140"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B83:E83"/>
+  <mergeCells count="36">
+    <mergeCell ref="B347:D347"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="B178:E178"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B318:E318"/>
+    <mergeCell ref="B327:D327"/>
+    <mergeCell ref="B295:E295"/>
+    <mergeCell ref="B275:E275"/>
+    <mergeCell ref="B227:D227"/>
+    <mergeCell ref="B198:E198"/>
+    <mergeCell ref="B207:D207"/>
     <mergeCell ref="B149:D149"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="B72:D72"/>
@@ -4621,17 +4634,15 @@
     <mergeCell ref="B237:E237"/>
     <mergeCell ref="B264:D264"/>
     <mergeCell ref="B246:D246"/>
-    <mergeCell ref="B347:D347"/>
-    <mergeCell ref="B159:E159"/>
-    <mergeCell ref="B178:E178"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B318:E318"/>
-    <mergeCell ref="B327:D327"/>
-    <mergeCell ref="B295:E295"/>
-    <mergeCell ref="B275:E275"/>
-    <mergeCell ref="B227:D227"/>
-    <mergeCell ref="B198:E198"/>
-    <mergeCell ref="B207:D207"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B140:E140"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4659,9 +4670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4694,49 +4703,49 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;" validAge="&amp;CHAR(34)&amp;Schedules!D8&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Tdap" vaccineIds="123" validAge="7 years"/&gt;</v>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;" validAge="&amp;CHAR(34)&amp;Schedules!E8&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Tdap" vaccineIds="123, 110, 114, 113, 115, 116, 121, 2060, 111, 2070" validAge="7 years"/&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B9&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C9&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B10&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C10&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Assume Comp" vaccineIds="-110"/&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B10&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C10&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B11&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C11&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="12 Months Old" vaccineIds="-12"/&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B11&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C11&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B12&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C12&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="4 Years Old" vaccineIds="-4"/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B12&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C12&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B13&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C13&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="7 Years Old" vaccineIds="-7"/&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B16&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C16&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D16&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B17&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C17&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D17&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="12 Months Old" age="12 months" vaccineId="-12"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B17&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C17&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D17&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B18&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C18&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D18&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="4 Years Old" age="4 years" vaccineId="-4"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B18&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C18&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D18&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B19&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C19&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D19&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="7 Years Old" age="7 years" vaccineId="-7"/&gt;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made minor changes to the schedule, nearly ready for production
</commit_message>
<xml_diff>
--- a/schedules/Diphtheria.xlsx
+++ b/schedules/Diphtheria.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="158">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -489,6 +489,15 @@
   </si>
   <si>
     <t>123, 110, 114, 113, 115, 116, 121, 2060, 111, 2070</t>
+  </si>
+  <si>
+    <t>4 years -4 days</t>
+  </si>
+  <si>
+    <t>7 years -4 days</t>
+  </si>
+  <si>
+    <t>12 months -4 d</t>
   </si>
 </sst>
 </file>
@@ -1320,9 +1329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J354"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1616,7 +1623,7 @@
         <v>130</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="D17" s="12">
         <v>-12</v>
@@ -1638,7 +1645,7 @@
         <v>134</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="D18" s="12">
         <v>-4</v>
@@ -1660,7 +1667,7 @@
         <v>131</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="D19" s="12">
         <v>-7</v>
@@ -4607,17 +4614,15 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="36">
-    <mergeCell ref="B347:D347"/>
-    <mergeCell ref="B159:E159"/>
-    <mergeCell ref="B178:E178"/>
-    <mergeCell ref="B168:D168"/>
-    <mergeCell ref="B318:E318"/>
-    <mergeCell ref="B327:D327"/>
-    <mergeCell ref="B295:E295"/>
-    <mergeCell ref="B275:E275"/>
-    <mergeCell ref="B227:D227"/>
-    <mergeCell ref="B198:E198"/>
-    <mergeCell ref="B207:D207"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B140:E140"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
     <mergeCell ref="B149:D149"/>
     <mergeCell ref="B102:E102"/>
     <mergeCell ref="B72:D72"/>
@@ -4634,15 +4639,17 @@
     <mergeCell ref="B237:E237"/>
     <mergeCell ref="B264:D264"/>
     <mergeCell ref="B246:D246"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B140:E140"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="B347:D347"/>
+    <mergeCell ref="B159:E159"/>
+    <mergeCell ref="B178:E178"/>
+    <mergeCell ref="B168:D168"/>
+    <mergeCell ref="B318:E318"/>
+    <mergeCell ref="B327:D327"/>
+    <mergeCell ref="B295:E295"/>
+    <mergeCell ref="B275:E275"/>
+    <mergeCell ref="B227:D227"/>
+    <mergeCell ref="B198:E198"/>
+    <mergeCell ref="B207:D207"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4670,7 +4677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A217"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A191" workbookViewId="0">
+      <selection sqref="A1:A217"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4734,19 +4743,19 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B17&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C17&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D17&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;transition name="12 Months Old" age="12 months" vaccineId="-12"/&gt;</v>
+        <v xml:space="preserve">  &lt;transition name="12 Months Old" age="12 months -4 d" vaccineId="-12"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B18&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C18&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D18&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;transition name="4 Years Old" age="4 years" vaccineId="-4"/&gt;</v>
+        <v xml:space="preserve">  &lt;transition name="4 Years Old" age="4 years -4 days" vaccineId="-4"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B19&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C19&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D19&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;transition name="7 Years Old" age="7 years" vaccineId="-7"/&gt;</v>
+        <v xml:space="preserve">  &lt;transition name="7 Years Old" age="7 years -4 days" vaccineId="-7"/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated T1 dose state
</commit_message>
<xml_diff>
--- a/schedules/Diphtheria.xlsx
+++ b/schedules/Diphtheria.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbkerr\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="6375"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12072"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$356</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$K$358</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="159">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t>12 months -4 d</t>
+  </si>
+  <si>
+    <t>Patient has not received pertussis vaccine (Tdap) after 7 years of age, Tdap due at 11 years of age.</t>
   </si>
 </sst>
 </file>
@@ -934,22 +937,22 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>120495</xdr:rowOff>
+      <xdr:rowOff>161147</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="https://documents.lucidchart.com/documents/eeb3fa82-6abd-49c0-85a7-09cbbaa842e0/pages/0_0?a=5953&amp;x=189&amp;y=68&amp;w=1565&amp;h=1144&amp;store=1&amp;accept=image%2F*&amp;auth=LCA%20c6dc249f3db1b3014559ac34660d27e17e8bab2e-ts%3D1466689900"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -960,18 +963,29 @@
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="85725" y="3076575"/>
-          <a:ext cx="8143875" cy="6378420"/>
+          <a:off x="121920" y="3192780"/>
+          <a:ext cx="9029700" cy="6600047"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1327,32 +1341,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J355"/>
+  <dimension ref="B1:J357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="C353" sqref="C353"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
-    <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="14.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="11.5703125" style="1"/>
-    <col min="16" max="16" width="33.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" style="1" customWidth="1"/>
-    <col min="18" max="22" width="11.5703125" style="1"/>
-    <col min="23" max="23" width="6.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="3.28515625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="1.5546875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="11.5546875" style="1"/>
+    <col min="16" max="16" width="33.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="1" customWidth="1"/>
+    <col min="18" max="22" width="11.5546875" style="1"/>
+    <col min="23" max="23" width="6.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="3.33203125" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1382,7 @@
       <c r="I2" s="46"/>
       <c r="J2" s="46"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +1402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
         <v>7</v>
       </c>
@@ -1406,7 +1420,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -1420,7 +1434,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1440,7 +1454,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
         <v>30</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
       <c r="C9" s="48"/>
       <c r="D9" s="48"/>
@@ -1499,7 +1513,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>113</v>
       </c>
@@ -1519,7 +1533,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>130</v>
       </c>
@@ -1537,7 +1551,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>134</v>
       </c>
@@ -1555,7 +1569,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
         <v>131</v>
       </c>
@@ -1573,7 +1587,7 @@
         <v>2070</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F14" s="9" t="s">
         <v>15</v>
       </c>
@@ -1584,7 +1598,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="46" t="s">
         <v>127</v>
       </c>
@@ -1600,7 +1614,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>128</v>
       </c>
@@ -1620,7 +1634,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>130</v>
       </c>
@@ -1642,7 +1656,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>134</v>
       </c>
@@ -1664,7 +1678,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>131</v>
       </c>
@@ -1675,7 +1689,10 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>32</v>
       </c>
@@ -1689,7 +1706,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
         <v>37</v>
       </c>
@@ -1700,7 +1717,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
         <v>40</v>
       </c>
@@ -1708,7 +1725,7 @@
       <c r="D63" s="46"/>
       <c r="E63" s="46"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="15"/>
       <c r="C64" s="6" t="s">
         <v>41</v>
@@ -1720,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
         <v>44</v>
       </c>
@@ -1732,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
         <v>49</v>
       </c>
@@ -1742,7 +1759,7 @@
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
         <v>50</v>
       </c>
@@ -1752,7 +1769,7 @@
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="16" t="s">
         <v>51</v>
       </c>
@@ -1762,7 +1779,7 @@
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
         <v>54</v>
       </c>
@@ -1772,7 +1789,7 @@
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="16" t="s">
         <v>56</v>
       </c>
@@ -1782,7 +1799,7 @@
       </c>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="16" t="s">
         <v>57</v>
       </c>
@@ -1790,14 +1807,14 @@
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C72" s="46"/>
       <c r="D72" s="46"/>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
         <v>4</v>
       </c>
@@ -1814,7 +1831,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="12" t="s">
         <v>130</v>
       </c>
@@ -1827,7 +1844,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="12" t="s">
         <v>7</v>
       </c>
@@ -1838,7 +1855,7 @@
       <c r="E75" s="12"/>
       <c r="F75" s="18"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="12" t="s">
         <v>11</v>
       </c>
@@ -1851,7 +1868,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="16" t="s">
         <v>67</v>
       </c>
@@ -1859,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="16" t="s">
         <v>68</v>
       </c>
@@ -1867,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>32</v>
       </c>
@@ -1879,7 +1896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
         <v>39</v>
       </c>
@@ -1887,7 +1904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="46" t="s">
         <v>40</v>
       </c>
@@ -1895,7 +1912,7 @@
       <c r="D83" s="46"/>
       <c r="E83" s="46"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="15"/>
       <c r="C84" s="6" t="s">
         <v>41</v>
@@ -1907,7 +1924,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="16" t="s">
         <v>44</v>
       </c>
@@ -1921,7 +1938,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="16" t="s">
         <v>49</v>
       </c>
@@ -1929,7 +1946,7 @@
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="16" t="s">
         <v>50</v>
       </c>
@@ -1939,7 +1956,7 @@
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="16" t="s">
         <v>51</v>
       </c>
@@ -1949,7 +1966,7 @@
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="16" t="s">
         <v>54</v>
       </c>
@@ -1959,7 +1976,7 @@
       <c r="D89" s="12"/>
       <c r="E89" s="12"/>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="16" t="s">
         <v>56</v>
       </c>
@@ -1971,7 +1988,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="16" t="s">
         <v>57</v>
       </c>
@@ -1979,14 +1996,14 @@
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C92" s="46"/>
       <c r="D92" s="46"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2020,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="12" t="s">
         <v>131</v>
       </c>
@@ -2016,7 +2033,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="12" t="s">
         <v>7</v>
       </c>
@@ -2027,7 +2044,7 @@
       <c r="E95" s="12"/>
       <c r="F95" s="18"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="12" t="s">
         <v>11</v>
       </c>
@@ -2040,7 +2057,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="16" t="s">
         <v>67</v>
       </c>
@@ -2048,7 +2065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="16" t="s">
         <v>68</v>
       </c>
@@ -2056,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>32</v>
       </c>
@@ -2068,7 +2085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
         <v>62</v>
       </c>
@@ -2076,7 +2093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="46" t="s">
         <v>72</v>
       </c>
@@ -2084,7 +2101,7 @@
       <c r="D102" s="46"/>
       <c r="E102" s="46"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="15"/>
       <c r="C103" s="6" t="s">
         <v>41</v>
@@ -2096,7 +2113,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="16" t="s">
         <v>44</v>
       </c>
@@ -2110,7 +2127,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="16" t="s">
         <v>49</v>
       </c>
@@ -2118,7 +2135,7 @@
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="16" t="s">
         <v>50</v>
       </c>
@@ -2128,7 +2145,7 @@
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="16" t="s">
         <v>51</v>
       </c>
@@ -2138,7 +2155,7 @@
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="16" t="s">
         <v>54</v>
       </c>
@@ -2148,7 +2165,7 @@
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="16" t="s">
         <v>56</v>
       </c>
@@ -2160,7 +2177,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="16" t="s">
         <v>57</v>
       </c>
@@ -2168,14 +2185,14 @@
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C111" s="46"/>
       <c r="D111" s="46"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="6" t="s">
         <v>4</v>
       </c>
@@ -2192,7 +2209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
         <v>131</v>
       </c>
@@ -2205,7 +2222,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="12" t="s">
         <v>7</v>
       </c>
@@ -2218,7 +2235,7 @@
       <c r="E114" s="12"/>
       <c r="F114" s="18"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="12" t="s">
         <v>7</v>
       </c>
@@ -2231,7 +2248,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" s="12" t="s">
         <v>11</v>
       </c>
@@ -2244,7 +2261,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="16" t="s">
         <v>67</v>
       </c>
@@ -2252,7 +2269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="16" t="s">
         <v>68</v>
       </c>
@@ -2260,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="5" t="s">
         <v>32</v>
       </c>
@@ -2272,7 +2289,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="14" t="s">
         <v>71</v>
       </c>
@@ -2280,7 +2297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="46" t="s">
         <v>72</v>
       </c>
@@ -2288,7 +2305,7 @@
       <c r="D122" s="46"/>
       <c r="E122" s="46"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="15"/>
       <c r="C123" s="6" t="s">
         <v>41</v>
@@ -2300,7 +2317,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="16" t="s">
         <v>44</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="16" t="s">
         <v>49</v>
       </c>
@@ -2324,7 +2341,7 @@
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="16" t="s">
         <v>50</v>
       </c>
@@ -2334,7 +2351,7 @@
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="16" t="s">
         <v>51</v>
       </c>
@@ -2344,7 +2361,7 @@
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="16" t="s">
         <v>54</v>
       </c>
@@ -2354,7 +2371,7 @@
       <c r="D128" s="12"/>
       <c r="E128" s="12"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="16" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2383,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130" s="16" t="s">
         <v>57</v>
       </c>
@@ -2374,14 +2391,14 @@
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C131" s="46"/>
       <c r="D131" s="46"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132" s="6" t="s">
         <v>4</v>
       </c>
@@ -2398,7 +2415,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133" s="12" t="s">
         <v>134</v>
       </c>
@@ -2411,7 +2428,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" s="12" t="s">
         <v>7</v>
       </c>
@@ -2422,7 +2439,7 @@
       <c r="E134" s="12"/>
       <c r="F134" s="18"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="12" t="s">
         <v>11</v>
       </c>
@@ -2435,7 +2452,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="16" t="s">
         <v>67</v>
       </c>
@@ -2443,7 +2460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="16" t="s">
         <v>68</v>
       </c>
@@ -2451,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="5" t="s">
         <v>32</v>
       </c>
@@ -2463,7 +2480,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="14" t="s">
         <v>124</v>
       </c>
@@ -2471,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="46" t="s">
         <v>40</v>
       </c>
@@ -2479,7 +2496,7 @@
       <c r="D141" s="46"/>
       <c r="E141" s="46"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="15"/>
       <c r="C142" s="6" t="s">
         <v>41</v>
@@ -2491,7 +2508,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="16" t="s">
         <v>44</v>
       </c>
@@ -2503,7 +2520,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="16" t="s">
         <v>49</v>
       </c>
@@ -2513,7 +2530,7 @@
       <c r="D144" s="12"/>
       <c r="E144" s="12"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" s="16" t="s">
         <v>50</v>
       </c>
@@ -2523,7 +2540,7 @@
       <c r="D145" s="12"/>
       <c r="E145" s="12"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="16" t="s">
         <v>51</v>
       </c>
@@ -2533,7 +2550,7 @@
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" s="16" t="s">
         <v>54</v>
       </c>
@@ -2543,7 +2560,7 @@
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" s="16" t="s">
         <v>56</v>
       </c>
@@ -2553,7 +2570,7 @@
       </c>
       <c r="E148" s="12"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" s="16" t="s">
         <v>57</v>
       </c>
@@ -2561,14 +2578,14 @@
       <c r="D149" s="12"/>
       <c r="E149" s="12"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C150" s="46"/>
       <c r="D150" s="46"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" s="6" t="s">
         <v>4</v>
       </c>
@@ -2585,7 +2602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" s="12" t="s">
         <v>131</v>
       </c>
@@ -2598,7 +2615,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153" s="12" t="s">
         <v>7</v>
       </c>
@@ -2609,7 +2626,7 @@
       <c r="E153" s="12"/>
       <c r="F153" s="18"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B154" s="12" t="s">
         <v>11</v>
       </c>
@@ -2622,7 +2639,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B155" s="16" t="s">
         <v>67</v>
       </c>
@@ -2630,7 +2647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B156" s="16" t="s">
         <v>68</v>
       </c>
@@ -2638,7 +2655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B158" s="5" t="s">
         <v>32</v>
       </c>
@@ -2650,7 +2667,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B159" s="14" t="s">
         <v>118</v>
       </c>
@@ -2658,7 +2675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B160" s="46" t="s">
         <v>72</v>
       </c>
@@ -2666,7 +2683,7 @@
       <c r="D160" s="46"/>
       <c r="E160" s="46"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="15"/>
       <c r="C161" s="6" t="s">
         <v>41</v>
@@ -2678,7 +2695,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162" s="16" t="s">
         <v>44</v>
       </c>
@@ -2690,7 +2707,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="16" t="s">
         <v>49</v>
       </c>
@@ -2698,7 +2715,7 @@
       <c r="D163" s="12"/>
       <c r="E163" s="12"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164" s="16" t="s">
         <v>50</v>
       </c>
@@ -2708,7 +2725,7 @@
       </c>
       <c r="E164" s="12"/>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165" s="16" t="s">
         <v>51</v>
       </c>
@@ -2718,7 +2735,7 @@
       </c>
       <c r="E165" s="12"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166" s="16" t="s">
         <v>54</v>
       </c>
@@ -2728,7 +2745,7 @@
       <c r="D166" s="12"/>
       <c r="E166" s="12"/>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="16" t="s">
         <v>56</v>
       </c>
@@ -2740,7 +2757,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168" s="16" t="s">
         <v>57</v>
       </c>
@@ -2748,14 +2765,14 @@
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C169" s="46"/>
       <c r="D169" s="46"/>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B170" s="6" t="s">
         <v>4</v>
       </c>
@@ -2772,7 +2789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="171" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B171" s="12" t="s">
         <v>131</v>
       </c>
@@ -2785,7 +2802,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B172" s="12" t="s">
         <v>7</v>
       </c>
@@ -2796,7 +2813,7 @@
       <c r="E172" s="12"/>
       <c r="F172" s="18"/>
     </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B173" s="12" t="s">
         <v>11</v>
       </c>
@@ -2807,7 +2824,7 @@
       <c r="E173" s="12"/>
       <c r="F173" s="18"/>
     </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B174" s="16" t="s">
         <v>67</v>
       </c>
@@ -2815,7 +2832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B175" s="16" t="s">
         <v>68</v>
       </c>
@@ -2823,7 +2840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177" s="5" t="s">
         <v>32</v>
       </c>
@@ -2835,7 +2852,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="14" t="s">
         <v>135</v>
       </c>
@@ -2843,7 +2860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B179" s="46" t="s">
         <v>72</v>
       </c>
@@ -2851,7 +2868,7 @@
       <c r="D179" s="46"/>
       <c r="E179" s="46"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="15"/>
       <c r="C180" s="6" t="s">
         <v>41</v>
@@ -2863,7 +2880,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B181" s="16" t="s">
         <v>44</v>
       </c>
@@ -2875,7 +2892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B182" s="16" t="s">
         <v>49</v>
       </c>
@@ -2883,7 +2900,7 @@
       <c r="D182" s="12"/>
       <c r="E182" s="12"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B183" s="16" t="s">
         <v>50</v>
       </c>
@@ -2893,7 +2910,7 @@
       </c>
       <c r="E183" s="12"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B184" s="16" t="s">
         <v>51</v>
       </c>
@@ -2903,7 +2920,7 @@
       </c>
       <c r="E184" s="12"/>
     </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B185" s="16" t="s">
         <v>54</v>
       </c>
@@ -2913,7 +2930,7 @@
       <c r="D185" s="12"/>
       <c r="E185" s="12"/>
     </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B186" s="16" t="s">
         <v>56</v>
       </c>
@@ -2925,7 +2942,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B187" s="16" t="s">
         <v>57</v>
       </c>
@@ -2933,14 +2950,14 @@
       <c r="D187" s="12"/>
       <c r="E187" s="12"/>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B188" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C188" s="46"/>
       <c r="D188" s="46"/>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B189" s="6" t="s">
         <v>4</v>
       </c>
@@ -2957,7 +2974,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B190" s="12" t="s">
         <v>131</v>
       </c>
@@ -2970,7 +2987,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B191" s="12" t="s">
         <v>7</v>
       </c>
@@ -2983,7 +3000,7 @@
       <c r="E191" s="12"/>
       <c r="F191" s="18"/>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B192" s="12" t="s">
         <v>7</v>
       </c>
@@ -2996,7 +3013,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B193" s="12" t="s">
         <v>11</v>
       </c>
@@ -3007,7 +3024,7 @@
       <c r="E193" s="12"/>
       <c r="F193" s="18"/>
     </row>
-    <row r="194" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B194" s="16" t="s">
         <v>67</v>
       </c>
@@ -3015,7 +3032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="195" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B195" s="16" t="s">
         <v>68</v>
       </c>
@@ -3023,7 +3040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B197" s="45" t="s">
         <v>32</v>
       </c>
@@ -3035,7 +3052,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B198" s="14" t="s">
         <v>150</v>
       </c>
@@ -3043,7 +3060,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B199" s="46" t="s">
         <v>72</v>
       </c>
@@ -3051,7 +3068,7 @@
       <c r="D199" s="46"/>
       <c r="E199" s="46"/>
     </row>
-    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B200" s="15"/>
       <c r="C200" s="6" t="s">
         <v>41</v>
@@ -3063,7 +3080,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B201" s="16" t="s">
         <v>44</v>
       </c>
@@ -3077,7 +3094,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B202" s="16" t="s">
         <v>49</v>
       </c>
@@ -3085,7 +3102,7 @@
       <c r="D202" s="12"/>
       <c r="E202" s="12"/>
     </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B203" s="16" t="s">
         <v>50</v>
       </c>
@@ -3095,7 +3112,7 @@
       <c r="D203" s="12"/>
       <c r="E203" s="12"/>
     </row>
-    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B204" s="16" t="s">
         <v>51</v>
       </c>
@@ -3105,7 +3122,7 @@
       <c r="D204" s="12"/>
       <c r="E204" s="12"/>
     </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B205" s="16" t="s">
         <v>54</v>
       </c>
@@ -3115,7 +3132,7 @@
       <c r="D205" s="12"/>
       <c r="E205" s="12"/>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B206" s="16" t="s">
         <v>56</v>
       </c>
@@ -3127,7 +3144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B207" s="16" t="s">
         <v>57</v>
       </c>
@@ -3135,14 +3152,14 @@
       <c r="D207" s="12"/>
       <c r="E207" s="12"/>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B208" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C208" s="46"/>
       <c r="D208" s="46"/>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B209" s="6" t="s">
         <v>4</v>
       </c>
@@ -3159,7 +3176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B210" s="12" t="s">
         <v>131</v>
       </c>
@@ -3172,7 +3189,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B211" s="12" t="s">
         <v>7</v>
       </c>
@@ -3183,7 +3200,7 @@
       <c r="E211" s="12"/>
       <c r="F211" s="18"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B212" s="12" t="s">
         <v>11</v>
       </c>
@@ -3196,7 +3213,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B213" s="16" t="s">
         <v>67</v>
       </c>
@@ -3204,7 +3221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B214" s="16" t="s">
         <v>68</v>
       </c>
@@ -3212,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B216" s="5" t="s">
         <v>32</v>
       </c>
@@ -3224,7 +3241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B217" s="14" t="s">
         <v>119</v>
       </c>
@@ -3232,7 +3249,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B218" s="46" t="s">
         <v>72</v>
       </c>
@@ -3240,7 +3257,7 @@
       <c r="D218" s="46"/>
       <c r="E218" s="46"/>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B219" s="15"/>
       <c r="C219" s="6" t="s">
         <v>41</v>
@@ -3252,7 +3269,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B220" s="16" t="s">
         <v>44</v>
       </c>
@@ -3266,7 +3283,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="221" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B221" s="16" t="s">
         <v>49</v>
       </c>
@@ -3274,7 +3291,7 @@
       <c r="D221" s="12"/>
       <c r="E221" s="12"/>
     </row>
-    <row r="222" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B222" s="16" t="s">
         <v>50</v>
       </c>
@@ -3284,7 +3301,7 @@
       <c r="D222" s="12"/>
       <c r="E222" s="12"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B223" s="16" t="s">
         <v>116</v>
       </c>
@@ -3294,7 +3311,7 @@
       <c r="D223" s="12"/>
       <c r="E223" s="12"/>
     </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B224" s="16" t="s">
         <v>51</v>
       </c>
@@ -3304,7 +3321,7 @@
       <c r="D224" s="12"/>
       <c r="E224" s="12"/>
     </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B225" s="16" t="s">
         <v>54</v>
       </c>
@@ -3314,7 +3331,7 @@
       <c r="D225" s="12"/>
       <c r="E225" s="12"/>
     </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B226" s="16" t="s">
         <v>56</v>
       </c>
@@ -3326,7 +3343,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B227" s="16" t="s">
         <v>57</v>
       </c>
@@ -3334,14 +3351,14 @@
       <c r="D227" s="12"/>
       <c r="E227" s="12"/>
     </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B228" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C228" s="46"/>
       <c r="D228" s="46"/>
     </row>
-    <row r="229" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B229" s="6" t="s">
         <v>4</v>
       </c>
@@ -3358,7 +3375,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="230" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B230" s="12" t="s">
         <v>131</v>
       </c>
@@ -3371,7 +3388,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="231" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B231" s="12" t="s">
         <v>7</v>
       </c>
@@ -3382,7 +3399,7 @@
       <c r="E231" s="12"/>
       <c r="F231" s="18"/>
     </row>
-    <row r="232" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B232" s="12" t="s">
         <v>11</v>
       </c>
@@ -3395,7 +3412,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B233" s="16" t="s">
         <v>67</v>
       </c>
@@ -3403,7 +3420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B234" s="16" t="s">
         <v>68</v>
       </c>
@@ -3411,7 +3428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B236" s="5" t="s">
         <v>32</v>
       </c>
@@ -3423,7 +3440,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B237" s="14" t="s">
         <v>84</v>
       </c>
@@ -3431,7 +3448,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B238" s="46" t="s">
         <v>72</v>
       </c>
@@ -3439,7 +3456,7 @@
       <c r="D238" s="46"/>
       <c r="E238" s="46"/>
     </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B239" s="15"/>
       <c r="C239" s="6" t="s">
         <v>41</v>
@@ -3451,7 +3468,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B240" s="16" t="s">
         <v>44</v>
       </c>
@@ -3463,7 +3480,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="241" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B241" s="16" t="s">
         <v>49</v>
       </c>
@@ -3471,7 +3488,7 @@
       <c r="D241" s="12"/>
       <c r="E241" s="12"/>
     </row>
-    <row r="242" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B242" s="16" t="s">
         <v>50</v>
       </c>
@@ -3481,7 +3498,7 @@
       </c>
       <c r="E242" s="12"/>
     </row>
-    <row r="243" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B243" s="16" t="s">
         <v>51</v>
       </c>
@@ -3491,7 +3508,7 @@
       </c>
       <c r="E243" s="12"/>
     </row>
-    <row r="244" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B244" s="16" t="s">
         <v>54</v>
       </c>
@@ -3501,7 +3518,7 @@
       <c r="D244" s="12"/>
       <c r="E244" s="12"/>
     </row>
-    <row r="245" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B245" s="16" t="s">
         <v>56</v>
       </c>
@@ -3513,7 +3530,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="246" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B246" s="16" t="s">
         <v>57</v>
       </c>
@@ -3521,14 +3538,14 @@
       <c r="D246" s="12"/>
       <c r="E246" s="12"/>
     </row>
-    <row r="247" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B247" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C247" s="46"/>
       <c r="D247" s="46"/>
     </row>
-    <row r="248" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B248" s="6" t="s">
         <v>4</v>
       </c>
@@ -3545,7 +3562,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="249" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B249" s="12" t="s">
         <v>7</v>
       </c>
@@ -3558,7 +3575,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="250" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B250" s="12" t="s">
         <v>11</v>
       </c>
@@ -3569,7 +3586,7 @@
       <c r="E250" s="12"/>
       <c r="F250" s="18"/>
     </row>
-    <row r="251" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B251" s="16" t="s">
         <v>67</v>
       </c>
@@ -3577,7 +3594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B252" s="16" t="s">
         <v>68</v>
       </c>
@@ -3585,7 +3602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B254" s="5" t="s">
         <v>32</v>
       </c>
@@ -3597,7 +3614,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="255" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B255" s="14" t="s">
         <v>110</v>
       </c>
@@ -3605,7 +3622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B256" s="46" t="s">
         <v>40</v>
       </c>
@@ -3613,7 +3630,7 @@
       <c r="D256" s="46"/>
       <c r="E256" s="46"/>
     </row>
-    <row r="257" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B257" s="15"/>
       <c r="C257" s="6" t="s">
         <v>41</v>
@@ -3625,7 +3642,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="258" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B258" s="16" t="s">
         <v>44</v>
       </c>
@@ -3637,7 +3654,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="259" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B259" s="16" t="s">
         <v>49</v>
       </c>
@@ -3645,7 +3662,7 @@
       <c r="D259" s="12"/>
       <c r="E259" s="12"/>
     </row>
-    <row r="260" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B260" s="16" t="s">
         <v>50</v>
       </c>
@@ -3655,7 +3672,7 @@
       <c r="D260" s="12"/>
       <c r="E260" s="12"/>
     </row>
-    <row r="261" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B261" s="16" t="s">
         <v>51</v>
       </c>
@@ -3665,7 +3682,7 @@
       <c r="D261" s="12"/>
       <c r="E261" s="12"/>
     </row>
-    <row r="262" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B262" s="16" t="s">
         <v>54</v>
       </c>
@@ -3675,7 +3692,7 @@
       <c r="D262" s="12"/>
       <c r="E262" s="12"/>
     </row>
-    <row r="263" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B263" s="16" t="s">
         <v>56</v>
       </c>
@@ -3685,7 +3702,7 @@
       </c>
       <c r="E263" s="12"/>
     </row>
-    <row r="264" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B264" s="16" t="s">
         <v>57</v>
       </c>
@@ -3693,14 +3710,14 @@
       <c r="D264" s="12"/>
       <c r="E264" s="12"/>
     </row>
-    <row r="265" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B265" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C265" s="46"/>
       <c r="D265" s="46"/>
     </row>
-    <row r="266" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B266" s="6" t="s">
         <v>4</v>
       </c>
@@ -3717,7 +3734,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="267" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B267" s="12" t="s">
         <v>7</v>
       </c>
@@ -3730,7 +3747,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="268" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B268" s="12" t="s">
         <v>11</v>
       </c>
@@ -3741,7 +3758,7 @@
       <c r="E268" s="12"/>
       <c r="F268" s="18"/>
     </row>
-    <row r="269" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B269" s="12" t="s">
         <v>113</v>
       </c>
@@ -3756,7 +3773,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="270" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B270" s="12" t="s">
         <v>113</v>
       </c>
@@ -3769,7 +3786,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="271" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B271" s="16" t="s">
         <v>67</v>
       </c>
@@ -3777,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B272" s="16" t="s">
         <v>68</v>
       </c>
@@ -3785,7 +3802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="274" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B274" s="5" t="s">
         <v>32</v>
       </c>
@@ -3797,7 +3814,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="275" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B275" s="14" t="s">
         <v>64</v>
       </c>
@@ -3805,7 +3822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B276" s="46" t="s">
         <v>72</v>
       </c>
@@ -3813,7 +3830,7 @@
       <c r="D276" s="46"/>
       <c r="E276" s="46"/>
     </row>
-    <row r="277" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B277" s="15"/>
       <c r="C277" s="6" t="s">
         <v>41</v>
@@ -3825,7 +3842,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="278" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B278" s="16" t="s">
         <v>44</v>
       </c>
@@ -3837,7 +3854,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="279" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B279" s="16" t="s">
         <v>49</v>
       </c>
@@ -3845,7 +3862,7 @@
       <c r="D279" s="12"/>
       <c r="E279" s="12"/>
     </row>
-    <row r="280" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B280" s="16" t="s">
         <v>50</v>
       </c>
@@ -3855,7 +3872,7 @@
       </c>
       <c r="E280" s="12"/>
     </row>
-    <row r="281" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B281" s="16" t="s">
         <v>51</v>
       </c>
@@ -3865,7 +3882,7 @@
       </c>
       <c r="E281" s="12"/>
     </row>
-    <row r="282" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B282" s="16" t="s">
         <v>54</v>
       </c>
@@ -3875,7 +3892,7 @@
       <c r="D282" s="12"/>
       <c r="E282" s="12"/>
     </row>
-    <row r="283" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B283" s="16" t="s">
         <v>56</v>
       </c>
@@ -3887,7 +3904,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="284" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B284" s="16" t="s">
         <v>57</v>
       </c>
@@ -3895,14 +3912,14 @@
       <c r="D284" s="12"/>
       <c r="E284" s="12"/>
     </row>
-    <row r="285" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B285" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C285" s="46"/>
       <c r="D285" s="46"/>
     </row>
-    <row r="286" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B286" s="6" t="s">
         <v>4</v>
       </c>
@@ -3919,7 +3936,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="287" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B287" s="12" t="s">
         <v>7</v>
       </c>
@@ -3932,7 +3949,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="288" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B288" s="12" t="s">
         <v>11</v>
       </c>
@@ -3943,7 +3960,7 @@
       <c r="E288" s="12"/>
       <c r="F288" s="18"/>
     </row>
-    <row r="289" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B289" s="12" t="s">
         <v>113</v>
       </c>
@@ -3958,7 +3975,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="290" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B290" s="12" t="s">
         <v>113</v>
       </c>
@@ -3971,7 +3988,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="291" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B291" s="16" t="s">
         <v>67</v>
       </c>
@@ -3979,7 +3996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B292" s="16" t="s">
         <v>68</v>
       </c>
@@ -3987,7 +4004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="294" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B294" s="5" t="s">
         <v>32</v>
       </c>
@@ -3999,7 +4016,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="295" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B295" s="14" t="s">
         <v>77</v>
       </c>
@@ -4007,7 +4024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B296" s="46" t="s">
         <v>72</v>
       </c>
@@ -4015,7 +4032,7 @@
       <c r="D296" s="46"/>
       <c r="E296" s="46"/>
     </row>
-    <row r="297" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B297" s="15"/>
       <c r="C297" s="6" t="s">
         <v>41</v>
@@ -4027,7 +4044,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="298" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B298" s="16" t="s">
         <v>44</v>
       </c>
@@ -4041,7 +4058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="299" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B299" s="16" t="s">
         <v>49</v>
       </c>
@@ -4049,7 +4066,7 @@
       <c r="D299" s="12"/>
       <c r="E299" s="12"/>
     </row>
-    <row r="300" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B300" s="16" t="s">
         <v>50</v>
       </c>
@@ -4059,7 +4076,7 @@
       </c>
       <c r="E300" s="12"/>
     </row>
-    <row r="301" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B301" s="16" t="s">
         <v>51</v>
       </c>
@@ -4069,7 +4086,7 @@
       </c>
       <c r="E301" s="12"/>
     </row>
-    <row r="302" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B302" s="16" t="s">
         <v>54</v>
       </c>
@@ -4079,7 +4096,7 @@
       <c r="D302" s="12"/>
       <c r="E302" s="12"/>
     </row>
-    <row r="303" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B303" s="16" t="s">
         <v>56</v>
       </c>
@@ -4091,7 +4108,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="304" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B304" s="16" t="s">
         <v>57</v>
       </c>
@@ -4099,14 +4116,14 @@
       <c r="D304" s="12"/>
       <c r="E304" s="12"/>
     </row>
-    <row r="305" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B305" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C305" s="46"/>
       <c r="D305" s="46"/>
     </row>
-    <row r="306" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B306" s="6" t="s">
         <v>4</v>
       </c>
@@ -4123,7 +4140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="307" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B307" s="12" t="s">
         <v>7</v>
       </c>
@@ -4138,7 +4155,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="308" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B308" s="12" t="s">
         <v>11</v>
       </c>
@@ -4151,7 +4168,7 @@
       </c>
       <c r="F308" s="18"/>
     </row>
-    <row r="309" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B309" s="12" t="s">
         <v>30</v>
       </c>
@@ -4162,7 +4179,7 @@
       <c r="E309" s="12"/>
       <c r="F309" s="18"/>
     </row>
-    <row r="310" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B310" s="12" t="s">
         <v>113</v>
       </c>
@@ -4177,7 +4194,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="311" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B311" s="12" t="s">
         <v>7</v>
       </c>
@@ -4190,7 +4207,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="312" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B312" s="12" t="s">
         <v>11</v>
       </c>
@@ -4203,7 +4220,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="313" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B313" s="12" t="s">
         <v>113</v>
       </c>
@@ -4216,7 +4233,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="314" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B314" s="16" t="s">
         <v>67</v>
       </c>
@@ -4224,7 +4241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B315" s="16" t="s">
         <v>68</v>
       </c>
@@ -4232,7 +4249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B317" s="5" t="s">
         <v>32</v>
       </c>
@@ -4244,7 +4261,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="318" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B318" s="14" t="s">
         <v>125</v>
       </c>
@@ -4252,7 +4269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="319" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B319" s="46" t="s">
         <v>72</v>
       </c>
@@ -4260,7 +4277,7 @@
       <c r="D319" s="46"/>
       <c r="E319" s="46"/>
     </row>
-    <row r="320" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B320" s="15"/>
       <c r="C320" s="6" t="s">
         <v>41</v>
@@ -4272,7 +4289,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="321" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B321" s="16" t="s">
         <v>44</v>
       </c>
@@ -4284,7 +4301,7 @@
       </c>
       <c r="E321" s="12"/>
     </row>
-    <row r="322" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B322" s="16" t="s">
         <v>49</v>
       </c>
@@ -4292,7 +4309,7 @@
       <c r="D322" s="12"/>
       <c r="E322" s="12"/>
     </row>
-    <row r="323" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B323" s="16" t="s">
         <v>50</v>
       </c>
@@ -4302,7 +4319,7 @@
       <c r="D323" s="12"/>
       <c r="E323" s="12"/>
     </row>
-    <row r="324" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B324" s="16" t="s">
         <v>51</v>
       </c>
@@ -4312,7 +4329,7 @@
       <c r="D324" s="12"/>
       <c r="E324" s="12"/>
     </row>
-    <row r="325" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B325" s="16" t="s">
         <v>54</v>
       </c>
@@ -4322,7 +4339,7 @@
       <c r="D325" s="12"/>
       <c r="E325" s="12"/>
     </row>
-    <row r="326" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B326" s="16" t="s">
         <v>56</v>
       </c>
@@ -4332,7 +4349,7 @@
       </c>
       <c r="E326" s="12"/>
     </row>
-    <row r="327" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B327" s="16" t="s">
         <v>57</v>
       </c>
@@ -4340,14 +4357,14 @@
       <c r="D327" s="12"/>
       <c r="E327" s="12"/>
     </row>
-    <row r="328" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B328" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C328" s="46"/>
       <c r="D328" s="46"/>
     </row>
-    <row r="329" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B329" s="6" t="s">
         <v>4</v>
       </c>
@@ -4364,7 +4381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="330" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B330" s="12" t="s">
         <v>11</v>
       </c>
@@ -4377,7 +4394,7 @@
       </c>
       <c r="F330" s="18"/>
     </row>
-    <row r="331" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="331" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B331" s="12" t="s">
         <v>30</v>
       </c>
@@ -4388,7 +4405,7 @@
       <c r="E331" s="12"/>
       <c r="F331" s="18"/>
     </row>
-    <row r="332" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B332" s="12" t="s">
         <v>7</v>
       </c>
@@ -4401,7 +4418,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="333" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B333" s="12" t="s">
         <v>11</v>
       </c>
@@ -4414,7 +4431,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="334" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B334" s="16" t="s">
         <v>67</v>
       </c>
@@ -4422,7 +4439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="335" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B335" s="16" t="s">
         <v>68</v>
       </c>
@@ -4430,7 +4447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="337" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B337" s="5" t="s">
         <v>32</v>
       </c>
@@ -4442,7 +4459,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="338" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B338" s="14" t="s">
         <v>139</v>
       </c>
@@ -4450,7 +4467,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="339" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B339" s="46" t="s">
         <v>72</v>
       </c>
@@ -4458,7 +4475,7 @@
       <c r="D339" s="46"/>
       <c r="E339" s="46"/>
     </row>
-    <row r="340" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B340" s="15"/>
       <c r="C340" s="6" t="s">
         <v>41</v>
@@ -4470,7 +4487,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="341" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B341" s="16" t="s">
         <v>44</v>
       </c>
@@ -4482,7 +4499,7 @@
       </c>
       <c r="E341" s="12"/>
     </row>
-    <row r="342" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B342" s="16" t="s">
         <v>49</v>
       </c>
@@ -4490,7 +4507,7 @@
       <c r="D342" s="12"/>
       <c r="E342" s="12"/>
     </row>
-    <row r="343" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B343" s="16" t="s">
         <v>50</v>
       </c>
@@ -4500,7 +4517,7 @@
       <c r="D343" s="12"/>
       <c r="E343" s="12"/>
     </row>
-    <row r="344" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B344" s="16" t="s">
         <v>51</v>
       </c>
@@ -4510,7 +4527,7 @@
       <c r="D344" s="12"/>
       <c r="E344" s="12"/>
     </row>
-    <row r="345" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B345" s="16" t="s">
         <v>54</v>
       </c>
@@ -4520,7 +4537,7 @@
       <c r="D345" s="12"/>
       <c r="E345" s="12"/>
     </row>
-    <row r="346" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B346" s="16" t="s">
         <v>56</v>
       </c>
@@ -4530,7 +4547,7 @@
       </c>
       <c r="E346" s="12"/>
     </row>
-    <row r="347" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B347" s="16" t="s">
         <v>57</v>
       </c>
@@ -4538,14 +4555,14 @@
       <c r="D347" s="12"/>
       <c r="E347" s="12"/>
     </row>
-    <row r="348" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B348" s="46" t="s">
         <v>58</v>
       </c>
       <c r="C348" s="46"/>
       <c r="D348" s="46"/>
     </row>
-    <row r="349" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B349" s="6" t="s">
         <v>4</v>
       </c>
@@ -4562,7 +4579,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="350" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B350" s="12" t="s">
         <v>11</v>
       </c>
@@ -4575,7 +4592,7 @@
       </c>
       <c r="F350" s="18"/>
     </row>
-    <row r="351" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B351" s="12" t="s">
         <v>30</v>
       </c>
@@ -4586,45 +4603,75 @@
       <c r="E351" s="12"/>
       <c r="F351" s="18"/>
     </row>
-    <row r="352" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B352" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C352" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D352" s="12"/>
+        <v>139</v>
+      </c>
+      <c r="D352" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="E352" s="12"/>
       <c r="F352" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="353" spans="2:6" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="353" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B353" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C353" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D353" s="12"/>
+        <v>139</v>
+      </c>
+      <c r="D353" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="E353" s="12"/>
       <c r="F353" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="354" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B354" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C354" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D354" s="12"/>
+      <c r="E354" s="12"/>
+      <c r="F354" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="355" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B355" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C355" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D355" s="12"/>
+      <c r="E355" s="12"/>
+      <c r="F355" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="354" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B354" s="16" t="s">
+    <row r="356" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B356" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C354" s="12">
+      <c r="C356" s="12">
         <v>5</v>
       </c>
     </row>
-    <row r="355" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B355" s="16" t="s">
+    <row r="357" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B357" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C355" s="12">
+      <c r="C357" s="12">
         <v>3</v>
       </c>
     </row>
@@ -4692,1321 +4739,1333 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A218"/>
+  <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209"/>
+    <sheetView topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.28515625" customWidth="1"/>
+    <col min="1" max="1" width="106.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Diphtheria"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Child" vaccineIds="110, 112, 114, 115, 116, 2060, 111, 2070, 113, 121, 1150, 142"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Adult" vaccineIds="122, 124, 123"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Td" vaccineIds="122, 124"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;" validAge="&amp;CHAR(34)&amp;Schedules!E8&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Tdap" vaccineIds="123, 110, 114, 113, 115, 116, 121, 2060, 111, 2070" validAge="7 years"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B10&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C10&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Assume Comp" vaccineIds="-110"/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B11&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C11&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="12 Months Old" vaccineIds="-12"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B12&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C12&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="4 Years Old" vaccineIds="-4"/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B13&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C13&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="7 Years Old" vaccineIds="-7"/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B17&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C17&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D17&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="12 Months Old" age="12 months -4 d" vaccineId="-12"/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B18&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C18&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D18&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="4 Years Old" age="4 years -4 days" vaccineId="-4"/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B19&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C19&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D19&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="7 Years Old" age="7 years -4 days" vaccineId="-7"/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B62&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D62&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="2 months"&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C77&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C65&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D65&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E65&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 weeks" interval="" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C66&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D66&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E66&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="6 weeks" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C67&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D67&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E67&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="2 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C68&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D68&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E68&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="3 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C69&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D69&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E69&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E70&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D71&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B74&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F74&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="12 Months Old" schedule="P1a" age="" reason="Patient reached 12 months of age without receiving first DTaP, moving to alternate schedule." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B75&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C75&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F75&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E75&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P2" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B76&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C76&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D76&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F76&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E76&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B82&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P2" dose="2" indication="" label="4 months"&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="10 weeks" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="4 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C88&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="5 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A1" age="" reason="Patient reached 7 years of age without completing childhood series, moving adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P3" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B101&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P3" dose="3" indication="" label="6 months"&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="14 weeks" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A2" age="" reason="Patient reached 7 years of age without completing childhood series, moving to 2nd dose in adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B114&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D114&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F114&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E114&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P4" age="4 years" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="K4" age="" reason="Patient received 3rd valid dose after 4 years of age, now expecting final DTaP booster. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E120&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P4" dose="4" indication="" label="15-18 months"&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="4"/&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C124&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E124&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="12 months" interval="6 months" grace="2 months"/&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C125&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E125&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C126&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="15 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C127&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E127&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="19 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C128&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E129&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="6 months" grace="2 months"/&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B133&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F133&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="4 Years Old" schedule="K4" age="" reason="Patient reached 4 years of age without receiving 4th valid dose in primary series, moving to catchup dose expected for kindergarten. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B134&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F134&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="K5" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B135&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F135&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="K5" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B140&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C140&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1a" dose="1" indication="" label="1st catchup"&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C156&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C155&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E143&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 weeks" interval="" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="6 weeks" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="2 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D146&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E146&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="3 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D147&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E147&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D148&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D149&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B152&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C152&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D152&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F152&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E152&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A1" age="" reason="Patient reached 7 years of age without receiving one valid dose of DTaP, moving to adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B153&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C153&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D153&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F153&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E153&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P2a" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B154&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C154&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D154&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F154&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E154&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B159&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C159&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D159&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E158&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P2a" dose="2" indication="" label="2nd catchup"&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C175&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C174&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C162&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D162&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E162&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C163&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D163&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E163&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C164&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D164&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E164&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C165&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D165&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E165&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C166&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D166&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E166&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D167&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E167&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D168&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B171&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C171&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D171&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F171&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E171&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A2" age="" reason="Patient reached 7 years of age, only receiving one valid dose of DTaP after 12 months, moving to 2nd dose in adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B172&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C172&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D172&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F172&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E172&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P3a" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B173&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C173&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D173&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F173&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E173&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B178&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C178&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D178&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E177&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P3a" dose="3" indication="" label="3rd catchup"&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C195&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C194&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C181&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D181&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E181&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C182&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D182&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E182&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C183&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D183&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E183&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C184&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D184&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E184&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C185&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D185&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E185&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D186&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E186&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D187&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B190&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C190&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D190&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F190&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E190&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A3" age="" reason="Patient reached 7 years of age, only receiving two valid doses of DTaP after 12 months, moving to 3rd dose in adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B191&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C191&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D191&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F191&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E191&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="P4" age="4 years" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B192&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C192&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D192&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F192&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E192&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="K4" age="" reason="Patient received 3rd valid dose after 4 years of age, now expecting final DTaP booster. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B193&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C193&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D193&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F193&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E193&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="INVALID" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B198&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C198&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D198&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E197&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="K4" dose="B" indication="" label="catchup kindegarten booster"&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C214&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C213&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="4"/&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C201&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D201&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E201&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="4 years" interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C202&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D202&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E202&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C203&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D203&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E203&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="4 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C204&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D204&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E204&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="4 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C205&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D205&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E205&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D206&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E206&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D207&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B210&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C210&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D210&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F210&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E210&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A3" age="" reason="Patient reached 7 years of age without receiving kindergarten booster after age 4 years, moving to 3rd dose in adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B211&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C211&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D211&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F211&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E211&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="T1" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B212&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C212&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D212&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F212&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E212&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="T1" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B217&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C217&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D217&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E216&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="K5" dose="B" indication="" label="kindegarten booster"&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C234&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C233&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="5"/&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C220&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D220&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E220&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="4 years" interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C221&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D221&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E221&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C222&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D222&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E222&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="4 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="20" t="str">
         <f>"    &lt;earlyOverdue age="&amp;CHAR(34)&amp;Schedules!C223&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D223&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E223&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;earlyOverdue age="6 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C224&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D224&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E224&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C225&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D225&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E225&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D226&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E226&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D227&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B230&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C230&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D230&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F230&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E230&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="7 Years Old" schedule="A3" age="" reason="Patient reached 7 years of age without receiving kindergarten booster after age 4 years, moving to 3rd dose in adult catchup schedule. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B231&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C231&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D231&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F231&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E231&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="T1" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B232&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C232&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D232&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F232&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E232&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="T1" age="" reason="Td or Tdap should not be given before 7 years of age. " historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B237&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C237&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D237&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E236&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="B10" dose="B" indication="" label="10-year booster"&gt;</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C252&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C251&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="4" column="4"/&gt;</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C240&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D240&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E240&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="5 years" grace="5 years"/&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C241&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D241&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E241&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C242&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D242&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E242&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="10 years" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C243&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D243&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E243&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="11 years" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C244&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D244&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E244&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D245&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E245&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="5 years" grace="5 years"/&gt;</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D246&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B249&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C249&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D249&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F249&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E249&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="B10" age="" reason="Child vaccine should not be given has booster." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B250&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C250&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D250&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F250&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E250&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="B10" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B255&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C255&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D255&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E254&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A1" dose="1" indication="" label="1st adult"&gt;</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C272&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C271&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C258&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D258&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E258&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="7 years" interval="" grace="0 days"/&gt;</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C259&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D259&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E259&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C260&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D260&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E260&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C261&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D261&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E261&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C262&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D262&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E262&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D263&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E263&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D264&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B267&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C267&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D267&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F267&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E267&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="A2" age="" reason="Child vaccine should not be given after 7 years of age." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B268&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C268&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D268&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F268&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E268&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="A2" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B269&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C269&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D269&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F269&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E269&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="B10" age="" reason="Tdap already given, and assuming adult received full DTaP series as a child, moving to 10 year booster schedule." historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B270&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C270&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D270&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F270&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E270&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="TN" age="" reason="Assuming adult received full DTaP series as a child but now needs to receive Tdap." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B275&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C275&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D275&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E274&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A2" dose="2" indication="" label="2nd adult"&gt;</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C292&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C291&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C278&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D278&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E278&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C279&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D279&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E279&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C280&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D280&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E280&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C281&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D281&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E281&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C282&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D282&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E282&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D283&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E283&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D284&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B287&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C287&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D287&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F287&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E287&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="A3" age="" reason="Child vaccine should not be given after 7 years of age." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B288&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C288&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D288&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F288&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E288&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="A3" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B289&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C289&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D289&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F289&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E289&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="B10" age="" reason="Tdap already given, and assuming adult received full DTaP series as a child, moving to 10 year booster schedule." historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B290&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C290&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D290&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F290&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E290&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="TN" age="" reason="Assuming adult received full DTaP series as a child but now needs to receive Tdap." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B295&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C295&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D295&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E294&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="A3" dose="3" indication="" label="3rd adult"&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C315&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C314&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C298&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D298&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E298&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="7 years" interval="6 months" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C299&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D299&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E299&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C300&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D300&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E300&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="6 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C301&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D301&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E301&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="6 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C302&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D302&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E302&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D303&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E303&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="6 months" grace="2 months"/&gt;</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D304&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B307&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C307&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D307&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F307&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E307&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="B10" age="" reason="Child vaccine should not be given after 7 years of age." historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B308&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C308&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D308&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F308&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E308&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="B10" age="" reason="" historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B309&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C309&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D309&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F309&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E309&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Tdap" schedule="B10" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B310&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C310&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D310&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F310&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E310&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="B10" age="" reason="Assuming adult received full DTaP series as a child, moving to 10 year booster schedule." historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B311&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C311&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D311&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F311&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E311&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="TN" age="" reason="Child vaccine should not be given after 7 years of age, Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B312&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C312&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D312&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F312&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E312&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="TN" age="" reason="Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B313&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C313&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D313&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F313&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E313&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Assume Comp" schedule="TN" age="" reason="Assuming adult received full DTaP series as a child but now needs to receive Tdap." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B318&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C318&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D318&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E317&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="TN" dose="B" indication="" label="Tdap Now"&gt;</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C335&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C334&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="4"/&gt;</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C321&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D321&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E321&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="7 years" interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C322&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D322&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E322&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C323&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D323&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E323&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C324&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D324&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E324&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C325&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D325&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E325&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D326&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E326&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D327&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B330&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C330&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D330&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F330&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E330&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="B10" age="" reason="" historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B331&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C331&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D331&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F331&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E331&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Tdap" schedule="B10" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B332&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C332&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D332&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F332&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E332&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="TN" age="" reason="Child vaccine should not be given after 7 years of age, Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B333&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C333&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D333&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F333&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E333&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="TN" age="" reason="Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B338&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C338&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D338&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E337&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="T1" dose="B" indication="" label="First Tdap"&gt;</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="19" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C355&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C354&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C357&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C356&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="5"/&gt;</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C341&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D341&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E341&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="7 years" interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C342&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D342&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E342&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C343&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D343&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E343&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="11 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C344&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D344&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E344&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="13 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C345&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D345&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E345&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A211" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D346&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E346&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A212" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D347&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B350&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C350&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D350&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F350&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E350&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="B10" age="" reason="" historyOfVaccineName="Tdap"/&gt;</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B351&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C351&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D351&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F351&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E351&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Tdap" schedule="B10" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B352&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C352&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D352&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F352&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E352&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="TN" age="" reason="Child vaccine should not be given after 7 years of age, Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="T1" age="11 years" reason="Patient has not received pertussis vaccine (Tdap) after 7 years of age, Tdap due at 11 years of age." historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A216" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B353&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C353&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D353&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F353&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E353&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="T1" age="11 years" reason="Patient has not received pertussis vaccine (Tdap) after 7 years of age, Tdap due at 11 years of age." historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="20" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B354&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C354&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D354&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F354&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E354&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Child" schedule="TN" age="" reason="Child vaccine should not be given after 7 years of age, Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="20" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B355&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C355&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D355&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F355&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E355&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Adult" schedule="TN" age="" reason="Tdap should be administered as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A217" s="20" t="str">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A218" s="19" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="19" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6027,31 +6086,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="1.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="22" customWidth="1"/>
     <col min="4" max="4" width="6" style="22" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="2.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" style="22" customWidth="1"/>
     <col min="8" max="8" width="6" style="22" customWidth="1"/>
     <col min="9" max="12" width="9" style="22" customWidth="1"/>
-    <col min="13" max="13" width="2.28515625" style="21" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="22" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="22" customWidth="1"/>
-    <col min="16" max="16" width="107.7109375" style="21" customWidth="1"/>
+    <col min="13" max="13" width="2.33203125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="7.44140625" style="22" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="107.6640625" style="21" customWidth="1"/>
     <col min="17" max="17" width="45" style="21" customWidth="1"/>
-    <col min="18" max="16384" width="11.5703125" style="21"/>
+    <col min="18" max="16384" width="11.5546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B1" s="23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>92</v>
       </c>
@@ -6091,7 +6150,7 @@
       </c>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>96</v>
       </c>
@@ -6131,7 +6190,7 @@
       </c>
       <c r="Q3" s="32"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="s">
         <v>98</v>
       </c>
@@ -6176,7 +6235,7 @@
       </c>
       <c r="Q4" s="32"/>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>99</v>
       </c>
@@ -6221,7 +6280,7 @@
       </c>
       <c r="Q5" s="32"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
         <v>100</v>
       </c>
@@ -6265,7 +6324,7 @@
       </c>
       <c r="Q6" s="32"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
         <v>101</v>
       </c>
@@ -6309,7 +6368,7 @@
       </c>
       <c r="Q7" s="32"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>102</v>
       </c>
@@ -6353,7 +6412,7 @@
       </c>
       <c r="Q8" s="32"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
         <v>103</v>
       </c>
@@ -6397,7 +6456,7 @@
       </c>
       <c r="Q9" s="32"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>104</v>
       </c>
@@ -6435,7 +6494,7 @@
       </c>
       <c r="Q10" s="32"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" s="33" t="s">
         <v>98</v>
       </c>
@@ -6478,7 +6537,7 @@
       </c>
       <c r="Q11" s="32"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
         <v>99</v>
       </c>
@@ -6521,7 +6580,7 @@
       </c>
       <c r="Q12" s="32"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="33" t="s">
         <v>100</v>
       </c>
@@ -6563,7 +6622,7 @@
       </c>
       <c r="Q13" s="32"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" s="33" t="s">
         <v>101</v>
       </c>
@@ -6605,7 +6664,7 @@
       </c>
       <c r="Q14" s="32"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>105</v>
       </c>
@@ -6641,7 +6700,7 @@
       </c>
       <c r="Q15" s="32"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="33" t="s">
         <v>98</v>
       </c>
@@ -6684,7 +6743,7 @@
       </c>
       <c r="Q16" s="32"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="33" t="s">
         <v>99</v>
       </c>
@@ -6726,7 +6785,7 @@
       </c>
       <c r="Q17" s="32"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
         <v>100</v>
       </c>
@@ -6754,7 +6813,7 @@
       </c>
       <c r="Q18" s="32"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>106</v>
       </c>
@@ -6786,7 +6845,7 @@
       </c>
       <c r="Q19" s="32"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="33" t="s">
         <v>98</v>
       </c>
@@ -6816,7 +6875,7 @@
       </c>
       <c r="Q20" s="32"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="33" t="s">
         <v>99</v>
       </c>
@@ -6846,7 +6905,7 @@
       </c>
       <c r="Q21" s="32"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="33" t="s">
         <v>100</v>
       </c>
@@ -6876,7 +6935,7 @@
       </c>
       <c r="Q22" s="32"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="33" t="s">
         <v>101</v>
       </c>
@@ -6904,7 +6963,7 @@
       </c>
       <c r="Q23" s="32"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
         <v>107</v>
       </c>
@@ -6925,7 +6984,7 @@
       </c>
       <c r="Q24" s="32"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
       <c r="C25" s="34"/>
       <c r="D25" s="10" t="str">
@@ -6947,7 +7006,7 @@
       </c>
       <c r="Q25" s="32"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -6962,7 +7021,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="32"/>
     </row>
-    <row r="27" spans="2:17" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>108</v>
       </c>
@@ -6979,7 +7038,7 @@
       <c r="O27" s="37"/>
       <c r="Q27" s="32"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>92</v>
       </c>
@@ -7015,7 +7074,7 @@
       </c>
       <c r="Q28" s="32"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
       <c r="C29" s="26"/>
       <c r="D29" s="27"/>
@@ -7036,7 +7095,7 @@
       </c>
       <c r="Q29" s="32"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="34"/>
       <c r="D30" s="10" t="str">
@@ -7063,7 +7122,7 @@
       </c>
       <c r="Q30" s="32"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
       <c r="C31" s="34"/>
       <c r="D31" s="10" t="str">
@@ -7100,7 +7159,7 @@
       </c>
       <c r="Q31" s="32"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="33"/>
       <c r="C32" s="34"/>
       <c r="D32" s="10">
@@ -7126,7 +7185,7 @@
       </c>
       <c r="Q32" s="32"/>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="36"/>
       <c r="D33" s="36"/>
       <c r="E33" s="37"/>
@@ -7140,7 +7199,7 @@
       <c r="O33" s="37"/>
       <c r="Q33" s="32"/>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34" s="36"/>
       <c r="D34" s="36"/>
       <c r="E34" s="37"/>
@@ -7154,7 +7213,7 @@
       <c r="O34" s="37"/>
       <c r="Q34" s="32"/>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35" s="36"/>
       <c r="D35" s="36"/>
       <c r="E35" s="37"/>
@@ -7168,7 +7227,7 @@
       <c r="O35" s="37"/>
       <c r="P35" s="32"/>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36" s="36"/>
       <c r="D36" s="36"/>
       <c r="E36" s="37"/>
@@ -7182,7 +7241,7 @@
       <c r="O36" s="37"/>
       <c r="P36" s="32"/>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37" s="36"/>
       <c r="D37" s="36"/>
       <c r="E37" s="37"/>
@@ -7196,7 +7255,7 @@
       <c r="O37" s="37"/>
       <c r="P37" s="32"/>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38" s="36"/>
       <c r="D38" s="36"/>
       <c r="E38" s="37"/>
@@ -7210,7 +7269,7 @@
       <c r="O38" s="37"/>
       <c r="P38" s="32"/>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39" s="36"/>
       <c r="D39" s="36"/>
       <c r="E39" s="37"/>
@@ -7224,7 +7283,7 @@
       <c r="O39" s="37"/>
       <c r="P39" s="32"/>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" s="36"/>
       <c r="D40" s="36"/>
       <c r="E40" s="37"/>
@@ -7238,7 +7297,7 @@
       <c r="O40" s="37"/>
       <c r="P40" s="32"/>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
       <c r="E41" s="37"/>
@@ -7252,7 +7311,7 @@
       <c r="O41" s="37"/>
       <c r="P41" s="32"/>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42" s="36"/>
       <c r="D42" s="36"/>
       <c r="E42" s="37"/>
@@ -7266,7 +7325,7 @@
       <c r="O42" s="37"/>
       <c r="P42" s="32"/>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C43" s="36"/>
       <c r="D43" s="36"/>
       <c r="E43" s="37"/>
@@ -7280,7 +7339,7 @@
       <c r="O43" s="36"/>
       <c r="P43" s="32"/>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C44" s="36"/>
       <c r="D44" s="36"/>
       <c r="E44" s="37"/>
@@ -7294,7 +7353,7 @@
       <c r="O44" s="37"/>
       <c r="P44" s="32"/>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C45" s="36"/>
       <c r="D45" s="36"/>
       <c r="E45" s="37"/>
@@ -7308,7 +7367,7 @@
       <c r="O45" s="37"/>
       <c r="Q45" s="32"/>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C46" s="36"/>
       <c r="D46" s="36"/>
       <c r="E46" s="37"/>

</xml_diff>